<commit_message>
updating with invoice for feb 2024
</commit_message>
<xml_diff>
--- a/2023.11 Invoicing/ethylene_oxide_invoice_total_through_November_2023.xlsx
+++ b/2023.11 Invoicing/ethylene_oxide_invoice_total_through_November_2023.xlsx
@@ -1,28 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattzabriskie/Library/CloudStorage/Box-Box/MattZ_Work/Shared Lab Space - Radiology/Ethylene Oxide Sterilizer/Consumables Invoicing/2023.11 Invoicing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattzabriskie/Desktop/Repos/eto_billing/2023.11 Invoicing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40195C9A-E16D-9847-B039-4C1F6E9184A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A2D780-B30D-8D40-9784-0508592C7A78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>PI_Account</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>PI</t>
   </si>
   <si>
     <t>Number Uses</t>
@@ -31,28 +47,49 @@
     <t>Total ($)</t>
   </si>
   <si>
-    <t>Alexander_Bridge</t>
+    <t>CL001</t>
   </si>
   <si>
     <t>Johnson</t>
   </si>
   <si>
-    <t>Hoareau</t>
-  </si>
-  <si>
-    <t>Shah/Rieke_UH3</t>
-  </si>
-  <si>
-    <t>Shah/Rieke_U18</t>
+    <t>CL002</t>
+  </si>
+  <si>
+    <t>Hoareau/Youngquist</t>
+  </si>
+  <si>
+    <t>CL003</t>
   </si>
   <si>
     <t>Palatinus</t>
   </si>
   <si>
-    <t>Youngquist</t>
+    <t>CL004</t>
+  </si>
+  <si>
+    <t>Silverton</t>
+  </si>
+  <si>
+    <t>CL005</t>
+  </si>
+  <si>
+    <t>Alexander</t>
+  </si>
+  <si>
+    <t>CL006</t>
   </si>
   <si>
     <t>Payne</t>
+  </si>
+  <si>
+    <t>CL007</t>
+  </si>
+  <si>
+    <t>Shah/Rieke</t>
+  </si>
+  <si>
+    <t>CL008</t>
   </si>
 </sst>
 </file>
@@ -416,20 +453,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -439,93 +477,120 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>1.7</v>
+      </c>
+      <c r="D2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>4.37</v>
+      </c>
+      <c r="D3">
+        <v>174.67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>0.7</v>
+      </c>
+      <c r="D4">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <v>0.2</v>
+      </c>
+      <c r="D7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>7.03</v>
+      </c>
+      <c r="D8">
+        <v>281.33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>1.7</v>
-      </c>
-      <c r="C3">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>3.83</v>
-      </c>
-      <c r="C4">
-        <v>153.33000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>7.03</v>
-      </c>
-      <c r="C5">
-        <v>281.33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="C6">
+      <c r="D9">
         <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>0.7</v>
-      </c>
-      <c r="C7">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>0.53</v>
-      </c>
-      <c r="C8">
-        <v>21.33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>0.2</v>
-      </c>
-      <c r="C9">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>